<commit_message>
update: Spectrum Viewer handles multiple waves supports shortcuts
Additional waves can be simply added by "Append to graph".
Added shortcuts: a, c, g, i, s, and t (These are common to some other windows.)
Modified shortcuts: ctrl+click, save -> add trace (Instead of just clicking, clicking with the ctrl key pressed to add traces.)
Removed shortcuts: click (This is changed to ctrl+click. Namely the shortcut to extract a wave at the displayed position was removed.)
</commit_message>
<xml_diff>
--- a/docs/source/shortcuts.xlsx
+++ b/docs/source/shortcuts.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Shortcuts</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Store spectrum on graph</t>
   </si>
   <si>
-    <t>Save spectrum as a wave</t>
-  </si>
-  <si>
     <t>Suppress live update</t>
   </si>
   <si>
@@ -137,10 +134,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>click</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>ctrl + click</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -416,6 +409,9 @@
   <si>
     <t>Close info bar (1D/2D/3D)</t>
     <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ctrl + click</t>
   </si>
 </sst>
 </file>
@@ -686,13 +682,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1002,7 +998,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1022,58 +1018,58 @@
     </row>
     <row r="2" spans="1:5" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="D3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="15"/>
+      <c r="A3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="D3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>6</v>
@@ -1081,13 +1077,13 @@
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>7</v>
@@ -1095,163 +1091,157 @@
     </row>
     <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D11" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
+        <v>41</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="15"/>
+        <v>44</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>3</v>
@@ -1259,7 +1249,7 @@
     </row>
     <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>4</v>
@@ -1268,7 +1258,7 @@
     <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="16"/>
+      <c r="B27" s="14"/>
     </row>
     <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1277,8 +1267,8 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.47244094488188981" right="0.47244094488188981" top="0.47244094488188981" bottom="0.47244094488188981" header="0" footer="0"/>

</xml_diff>